<commit_message>
2024 12 19 ajout du calcul massique
</commit_message>
<xml_diff>
--- a/bilan_carbone_export.xlsx
+++ b/bilan_carbone_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,16 @@
           <t>Émissions (kg CO₂e)</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Code NACRES</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Consommable</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -483,16 +493,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NA25</t>
+          <t>NB13</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Produits biochimiques courants (tampons, bsa, etc.)</t>
+          <t>Culture cellulaire eucaryote : consommables en plastique specifiques</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -500,404 +510,138 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>67.5</v>
+        <v>42</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NB13</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Tube Falcon 50ml</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Achats</t>
+          <t>Véhicules</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Consommables (Matières premières, produits chimiques/biologiques et organismes vivants)</t>
+          <t>Voiture</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NA71</t>
+          <t>Essence</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Serums et autres milieux pour culture de cellules animales</t>
+          <t>Voiture particulière, moyenne parc, motorisation essence</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>180</v>
+        <v>1000</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>euro</t>
+          <t>km</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>81</v>
+        <v>223.4</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Achats</t>
+          <t>Véhicules</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Consommables (Matières premières, produits chimiques/biologiques et organismes vivants)</t>
+          <t>ferroviaire</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NA73</t>
+          <t>TGV &gt; 200 km</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Milieux pour culture de petits organismes vivants</t>
+          <t>TGV</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>200</v>
+        <v>50000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>euro</t>
+          <t>km</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>90</v>
+        <v>165</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Achats</t>
+          <t>Machine</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Consommables (Matières premières, produits chimiques/biologiques et organismes vivants)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NB13</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Culture cellulaire eucaryote : consommables en plastique specifiques</t>
-        </is>
-      </c>
+          <t>COUCOU</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>780</v>
+        <v>30</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>euro</t>
+          <t>kWh</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>327.6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Achats</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Consommables (Matières premières, produits chimiques/biologiques et organismes vivants)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NB02</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Pointes (cones) pour micropipettes mono-canal et multi-canaux</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>euro</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Véhicules</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Voiture</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Diesel</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Voiture particulière , moyenne parc, motorisation gazole</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>3515</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>km</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>745.5315000000001</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Véhicules</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ferroviaire</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>TGV &gt; 200 km</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>TGV</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>111000</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>km</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>366.3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Incubateur</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>2628</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>kWh</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>1560.2436</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>centrifugeuse</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>180</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>kWh</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>106.866</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Autoclave</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
-        <v>150</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>kWh</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Machine</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Microscope</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>1920</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>kWh</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>99.84</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Activités agricoles</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Utilisation d'engrais</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>minerals</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Epandage d'engrais minéraux</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>kg d'azote</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>57.3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Infra. de recherche</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Astronomie</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>AAT</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Anglo-Australian Telescope</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>1e-05</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>% utilisation infra.</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>335.5180000000001</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Infra. de recherche</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Calcul GENCI</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>GPU puissant</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>GPU</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>heures.GPU</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>333.7</v>
+        <v>1.56</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>